<commit_message>
Add 121 DP approach
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Localdata\LeetCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF6EA2D-25D1-456E-9F8A-2FBC1E09FCB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="252">
   <si>
     <t>Question Number</t>
   </si>
@@ -290,10 +289,6 @@
   </si>
   <si>
     <t>OnePass, Brute,DP</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>Study DP approach</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
@@ -867,12 +862,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="41">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -880,7 +875,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -888,7 +883,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -901,7 +896,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF212121"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -967,7 +962,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -1206,8 +1201,8 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="超連結" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1518,24 +1513,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.81640625" customWidth="1"/>
-    <col min="3" max="3" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.81640625" customWidth="1"/>
-    <col min="9" max="9" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.796875" customWidth="1"/>
+    <col min="3" max="3" width="7.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.796875" customWidth="1"/>
+    <col min="9" max="9" width="10.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1564,7 +1559,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1584,13 +1579,13 @@
         <v>21</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1616,7 +1611,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1642,7 +1637,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1671,7 +1666,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>11</v>
       </c>
@@ -1697,7 +1692,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>15</v>
       </c>
@@ -1723,7 +1718,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>19</v>
       </c>
@@ -1749,7 +1744,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>20</v>
       </c>
@@ -1769,13 +1764,13 @@
         <v>34</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>21</v>
       </c>
@@ -1795,13 +1790,13 @@
         <v>36</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>23</v>
       </c>
@@ -1830,7 +1825,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>33</v>
       </c>
@@ -1856,7 +1851,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>39</v>
       </c>
@@ -1885,7 +1880,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>48</v>
       </c>
@@ -1914,7 +1909,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>49</v>
       </c>
@@ -1943,7 +1938,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>53</v>
       </c>
@@ -1972,7 +1967,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>54</v>
       </c>
@@ -1998,7 +1993,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>55</v>
       </c>
@@ -2027,7 +2022,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>56</v>
       </c>
@@ -2053,7 +2048,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>57</v>
       </c>
@@ -2079,7 +2074,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>59</v>
       </c>
@@ -2111,7 +2106,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>62</v>
       </c>
@@ -2143,7 +2138,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>70</v>
       </c>
@@ -2169,7 +2164,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>73</v>
       </c>
@@ -2201,7 +2196,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>76</v>
       </c>
@@ -2224,7 +2219,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>79</v>
       </c>
@@ -2256,7 +2251,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>91</v>
       </c>
@@ -2279,7 +2274,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>98</v>
       </c>
@@ -2311,7 +2306,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>94</v>
       </c>
@@ -2337,7 +2332,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>100</v>
       </c>
@@ -2366,7 +2361,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>102</v>
       </c>
@@ -2398,7 +2393,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>104</v>
       </c>
@@ -2424,7 +2419,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>105</v>
       </c>
@@ -2447,7 +2442,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>121</v>
       </c>
@@ -2467,21 +2462,18 @@
         <v>87</v>
       </c>
       <c r="G34">
-        <v>1</v>
-      </c>
-      <c r="H34" t="s">
-        <v>88</v>
+        <v>2</v>
       </c>
       <c r="I34" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>124</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
@@ -2496,12 +2488,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15">
+    <row r="36" spans="1:10" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>125</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C36" t="s">
         <v>20</v>
@@ -2510,7 +2502,7 @@
         <v>8</v>
       </c>
       <c r="E36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G36">
         <v>1</v>
@@ -2519,12 +2511,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>128</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C37" t="s">
         <v>20</v>
@@ -2539,204 +2531,204 @@
         <v>1</v>
       </c>
       <c r="H37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I37" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>133</v>
       </c>
       <c r="B38" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" t="s">
         <v>94</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" t="s">
         <v>95</v>
       </c>
-      <c r="D38" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>96</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38" t="s">
         <v>97</v>
       </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
+        <v>29</v>
+      </c>
+      <c r="J38" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="I38" t="s">
-        <v>29</v>
-      </c>
-      <c r="J38" s="15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>139</v>
       </c>
       <c r="B39" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" t="s">
         <v>100</v>
       </c>
-      <c r="C39" t="s">
-        <v>95</v>
-      </c>
-      <c r="D39" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>101</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
+        <v>103</v>
+      </c>
+      <c r="I39" t="s">
+        <v>29</v>
+      </c>
+      <c r="J39" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
-      <c r="H39" t="s">
-        <v>104</v>
-      </c>
-      <c r="I39" t="s">
-        <v>29</v>
-      </c>
-      <c r="J39" s="15" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>141</v>
       </c>
       <c r="B40" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" t="s">
         <v>105</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>106</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>107</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
+        <v>110</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="I40" t="s">
+        <v>29</v>
+      </c>
+      <c r="J40" t="s">
         <v>108</v>
       </c>
-      <c r="F40" t="s">
-        <v>111</v>
-      </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="I40" t="s">
-        <v>29</v>
-      </c>
-      <c r="J40" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>143</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D41" t="s">
+        <v>106</v>
+      </c>
+      <c r="E41" t="s">
         <v>107</v>
       </c>
-      <c r="E41" t="s">
-        <v>108</v>
-      </c>
       <c r="F41" t="s">
+        <v>111</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="I41" t="s">
+        <v>29</v>
+      </c>
+      <c r="J41" t="s">
         <v>112</v>
       </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-      <c r="I41" t="s">
-        <v>29</v>
-      </c>
-      <c r="J41" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>152</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" t="s">
         <v>114</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>115</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>116</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>117</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42" t="s">
         <v>118</v>
       </c>
-      <c r="G42">
-        <v>1</v>
-      </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
+        <v>29</v>
+      </c>
+      <c r="J42" t="s">
         <v>119</v>
       </c>
-      <c r="I42" t="s">
-        <v>29</v>
-      </c>
-      <c r="J42" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2114</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C43" t="s">
+        <v>105</v>
+      </c>
+      <c r="D43" t="s">
         <v>106</v>
-      </c>
-      <c r="D43" t="s">
-        <v>107</v>
       </c>
       <c r="E43" t="s">
         <v>24</v>
       </c>
       <c r="F43" t="s">
+        <v>121</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="J43" t="s">
         <v>122</v>
       </c>
-      <c r="G43">
-        <v>1</v>
-      </c>
-      <c r="J43" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2236</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C44" t="s">
+        <v>105</v>
+      </c>
+      <c r="D44" t="s">
         <v>106</v>
-      </c>
-      <c r="D44" t="s">
-        <v>107</v>
       </c>
       <c r="E44" t="s">
         <v>71</v>
@@ -2745,12 +2737,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1023</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
@@ -2765,15 +2757,15 @@
         <v>1</v>
       </c>
       <c r="J45" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>831</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
@@ -2788,15 +2780,15 @@
         <v>1</v>
       </c>
       <c r="J46" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>153</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
@@ -2814,18 +2806,18 @@
         <v>1</v>
       </c>
       <c r="H47" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I47" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>190</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C48" t="s">
         <v>20</v>
@@ -2834,7 +2826,7 @@
         <v>8</v>
       </c>
       <c r="E48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F48" t="s">
         <v>37</v>
@@ -2843,21 +2835,21 @@
         <v>1</v>
       </c>
       <c r="H48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I48" t="s">
         <v>29</v>
       </c>
       <c r="J48" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>191</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C49" t="s">
         <v>20</v>
@@ -2866,10 +2858,10 @@
         <v>8</v>
       </c>
       <c r="E49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G49">
         <v>1</v>
@@ -2878,12 +2870,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>198</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C50" t="s">
         <v>6</v>
@@ -2901,21 +2893,21 @@
         <v>1</v>
       </c>
       <c r="H50" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I50" t="s">
         <v>29</v>
       </c>
       <c r="J50" s="15" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>200</v>
       </c>
       <c r="B51" s="28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C51" t="s">
         <v>6</v>
@@ -2927,27 +2919,27 @@
         <v>9</v>
       </c>
       <c r="F51" t="s">
+        <v>139</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51" t="s">
         <v>140</v>
       </c>
-      <c r="G51">
-        <v>1</v>
-      </c>
-      <c r="H51" t="s">
-        <v>141</v>
-      </c>
       <c r="I51" t="s">
         <v>29</v>
       </c>
       <c r="J51" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>206</v>
       </c>
       <c r="B52" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C52" t="s">
         <v>20</v>
@@ -2959,24 +2951,24 @@
         <v>14</v>
       </c>
       <c r="F52" t="s">
+        <v>144</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="I52" t="s">
+        <v>29</v>
+      </c>
+      <c r="J52" t="s">
         <v>145</v>
       </c>
-      <c r="G52">
-        <v>1</v>
-      </c>
-      <c r="I52" t="s">
-        <v>29</v>
-      </c>
-      <c r="J52" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10">
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>207</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C53" t="s">
         <v>6</v>
@@ -2985,27 +2977,27 @@
         <v>8</v>
       </c>
       <c r="E53" t="s">
+        <v>146</v>
+      </c>
+      <c r="F53" t="s">
+        <v>139</v>
+      </c>
+      <c r="H53" t="s">
         <v>147</v>
       </c>
-      <c r="F53" t="s">
-        <v>140</v>
-      </c>
-      <c r="H53" t="s">
+      <c r="I53" t="s">
+        <v>29</v>
+      </c>
+      <c r="J53" t="s">
         <v>148</v>
       </c>
-      <c r="I53" t="s">
-        <v>29</v>
-      </c>
-      <c r="J53" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>208</v>
       </c>
       <c r="B54" s="29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
@@ -3014,24 +3006,24 @@
         <v>8</v>
       </c>
       <c r="E54" t="s">
+        <v>150</v>
+      </c>
+      <c r="H54" t="s">
         <v>151</v>
       </c>
-      <c r="H54" t="s">
+      <c r="I54" t="s">
+        <v>29</v>
+      </c>
+      <c r="J54" t="s">
         <v>152</v>
       </c>
-      <c r="I54" t="s">
-        <v>29</v>
-      </c>
-      <c r="J54" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>211</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C55" t="s">
         <v>6</v>
@@ -3040,98 +3032,98 @@
         <v>8</v>
       </c>
       <c r="E55" t="s">
+        <v>150</v>
+      </c>
+      <c r="H55" t="s">
         <v>151</v>
       </c>
-      <c r="H55" t="s">
-        <v>152</v>
-      </c>
       <c r="I55" t="s">
         <v>29</v>
       </c>
       <c r="J55" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>212</v>
       </c>
       <c r="B56" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" t="s">
         <v>157</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" t="s">
+        <v>150</v>
+      </c>
+      <c r="F56" t="s">
         <v>158</v>
       </c>
-      <c r="D56" t="s">
-        <v>8</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56" t="s">
         <v>151</v>
       </c>
-      <c r="F56" t="s">
+      <c r="I56" t="s">
+        <v>29</v>
+      </c>
+      <c r="J56" t="s">
         <v>159</v>
       </c>
-      <c r="G56">
-        <v>1</v>
-      </c>
-      <c r="H56" t="s">
-        <v>152</v>
-      </c>
-      <c r="I56" t="s">
-        <v>29</v>
-      </c>
-      <c r="J56" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>213</v>
       </c>
       <c r="B57" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="C57" t="s">
         <v>162</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>163</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>164</v>
       </c>
-      <c r="E57" t="s">
-        <v>165</v>
-      </c>
       <c r="G57">
         <v>1</v>
       </c>
       <c r="H57" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I57" t="s">
         <v>29</v>
       </c>
       <c r="J57" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>217</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C58" t="s">
+        <v>165</v>
+      </c>
+      <c r="D58" t="s">
         <v>166</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
+        <v>164</v>
+      </c>
+      <c r="F58" t="s">
         <v>167</v>
       </c>
-      <c r="E58" t="s">
-        <v>165</v>
-      </c>
-      <c r="F58" t="s">
-        <v>168</v>
-      </c>
       <c r="G58">
         <v>1</v>
       </c>
@@ -3139,147 +3131,147 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>226</v>
       </c>
       <c r="B59" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="C59" t="s">
         <v>170</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>171</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>172</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>173</v>
       </c>
-      <c r="F59" t="s">
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59" t="s">
         <v>174</v>
       </c>
-      <c r="G59">
-        <v>1</v>
-      </c>
-      <c r="H59" t="s">
+      <c r="I59" t="s">
+        <v>29</v>
+      </c>
+      <c r="J59" t="s">
         <v>175</v>
       </c>
-      <c r="I59" t="s">
-        <v>29</v>
-      </c>
-      <c r="J59" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10">
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>230</v>
       </c>
       <c r="B60" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="C60" t="s">
         <v>177</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>178</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>179</v>
       </c>
-      <c r="E60" t="s">
+      <c r="F60" t="s">
+        <v>173</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60" t="s">
         <v>180</v>
       </c>
-      <c r="F60" t="s">
-        <v>174</v>
-      </c>
-      <c r="G60">
-        <v>1</v>
-      </c>
-      <c r="H60" t="s">
-        <v>181</v>
-      </c>
       <c r="I60" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>235</v>
       </c>
       <c r="B61" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="C61" t="s">
         <v>182</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>183</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
+        <v>150</v>
+      </c>
+      <c r="F61" t="s">
+        <v>185</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="I61" t="s">
+        <v>29</v>
+      </c>
+      <c r="J61" t="s">
         <v>184</v>
       </c>
-      <c r="E61" t="s">
-        <v>151</v>
-      </c>
-      <c r="F61" t="s">
-        <v>186</v>
-      </c>
-      <c r="G61">
-        <v>1</v>
-      </c>
-      <c r="I61" t="s">
-        <v>29</v>
-      </c>
-      <c r="J61" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>238</v>
       </c>
       <c r="B62" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C62" t="s">
         <v>187</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
+        <v>106</v>
+      </c>
+      <c r="E62" t="s">
         <v>188</v>
       </c>
-      <c r="D62" t="s">
-        <v>107</v>
-      </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>189</v>
       </c>
-      <c r="F62" t="s">
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62" t="s">
         <v>190</v>
       </c>
-      <c r="G62">
-        <v>1</v>
-      </c>
-      <c r="H62" t="s">
+      <c r="I62" t="s">
+        <v>29</v>
+      </c>
+      <c r="J62" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="I62" t="s">
-        <v>29</v>
-      </c>
-      <c r="J62" s="10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>242</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C63" t="s">
         <v>194</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>195</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>196</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>197</v>
       </c>
-      <c r="F63" t="s">
-        <v>198</v>
-      </c>
       <c r="G63">
         <v>1</v>
       </c>
@@ -3287,15 +3279,15 @@
         <v>29</v>
       </c>
       <c r="J63" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>252</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C64" t="s">
         <v>20</v>
@@ -3310,21 +3302,21 @@
         <v>1</v>
       </c>
       <c r="H64" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I64" t="s">
         <v>29</v>
       </c>
       <c r="J64" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>253</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C65" t="s">
         <v>6</v>
@@ -3336,18 +3328,18 @@
         <v>9</v>
       </c>
       <c r="H65" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I65" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>261</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C66" t="s">
         <v>6</v>
@@ -3359,18 +3351,18 @@
         <v>71</v>
       </c>
       <c r="H66" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I66" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>268</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C67" t="s">
         <v>20</v>
@@ -3385,197 +3377,197 @@
         <v>1</v>
       </c>
       <c r="H67" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I67" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>269</v>
       </c>
       <c r="B68" s="36" t="s">
+        <v>204</v>
+      </c>
+      <c r="C68" t="s">
         <v>205</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>206</v>
       </c>
-      <c r="D68" t="s">
+      <c r="I68" t="s">
+        <v>29</v>
+      </c>
+      <c r="J68" t="s">
         <v>207</v>
       </c>
-      <c r="I68" t="s">
-        <v>29</v>
-      </c>
-      <c r="J68" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>271</v>
       </c>
       <c r="B69" s="36" t="s">
+        <v>209</v>
+      </c>
+      <c r="C69" t="s">
         <v>210</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>211</v>
       </c>
-      <c r="D69" t="s">
-        <v>212</v>
-      </c>
       <c r="I69" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>295</v>
       </c>
       <c r="B70" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="C70" t="s">
         <v>213</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>214</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
         <v>215</v>
       </c>
-      <c r="E70" t="s">
+      <c r="F70" t="s">
+        <v>217</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="I70" t="s">
+        <v>29</v>
+      </c>
+      <c r="J70" t="s">
         <v>216</v>
       </c>
-      <c r="F70" t="s">
-        <v>218</v>
-      </c>
-      <c r="G70">
-        <v>1</v>
-      </c>
-      <c r="I70" t="s">
-        <v>29</v>
-      </c>
-      <c r="J70" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10">
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>297</v>
       </c>
       <c r="B71" s="38" t="s">
+        <v>218</v>
+      </c>
+      <c r="C71" t="s">
+        <v>205</v>
+      </c>
+      <c r="D71" t="s">
         <v>219</v>
       </c>
-      <c r="C71" t="s">
-        <v>206</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>220</v>
       </c>
-      <c r="E71" t="s">
-        <v>221</v>
-      </c>
       <c r="I71" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>300</v>
       </c>
       <c r="B72" s="39" t="s">
+        <v>221</v>
+      </c>
+      <c r="C72" t="s">
         <v>222</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
         <v>223</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
         <v>224</v>
       </c>
-      <c r="E72" t="s">
+      <c r="F72" t="s">
         <v>225</v>
       </c>
-      <c r="F72" t="s">
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72" t="s">
+        <v>227</v>
+      </c>
+      <c r="I72" t="s">
+        <v>29</v>
+      </c>
+      <c r="J72" t="s">
         <v>226</v>
       </c>
-      <c r="G72">
-        <v>1</v>
-      </c>
-      <c r="H72" t="s">
-        <v>228</v>
-      </c>
-      <c r="I72" t="s">
-        <v>29</v>
-      </c>
-      <c r="J72" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10">
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>322</v>
       </c>
       <c r="B73" s="36" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C73" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D73" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E73" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F73" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G73">
         <v>1</v>
       </c>
       <c r="H73" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I73" t="s">
         <v>29</v>
       </c>
       <c r="J73" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>323</v>
       </c>
       <c r="B74" t="s">
+        <v>233</v>
+      </c>
+      <c r="C74" t="s">
+        <v>94</v>
+      </c>
+      <c r="D74" t="s">
+        <v>106</v>
+      </c>
+      <c r="E74" t="s">
+        <v>146</v>
+      </c>
+      <c r="F74" t="s">
         <v>234</v>
       </c>
-      <c r="C74" t="s">
-        <v>95</v>
-      </c>
-      <c r="D74" t="s">
-        <v>107</v>
-      </c>
-      <c r="E74" t="s">
-        <v>147</v>
-      </c>
-      <c r="F74" t="s">
+      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="I74" t="s">
+        <v>29</v>
+      </c>
+      <c r="J74" t="s">
         <v>235</v>
       </c>
-      <c r="G74">
-        <v>1</v>
-      </c>
-      <c r="I74" t="s">
-        <v>29</v>
-      </c>
-      <c r="J74" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10">
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>338</v>
       </c>
       <c r="B75" s="40" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C75" t="s">
         <v>20</v>
@@ -3584,7 +3576,7 @@
         <v>8</v>
       </c>
       <c r="E75" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F75" t="s">
         <v>26</v>
@@ -3593,21 +3585,21 @@
         <v>1</v>
       </c>
       <c r="H75" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I75" t="s">
         <v>29</v>
       </c>
       <c r="J75" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>347</v>
       </c>
       <c r="B76" s="41" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
@@ -3619,7 +3611,7 @@
         <v>9</v>
       </c>
       <c r="F76" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G76">
         <v>1</v>
@@ -3631,15 +3623,15 @@
         <v>29</v>
       </c>
       <c r="J76" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>371</v>
       </c>
       <c r="B77" s="41" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
@@ -3648,30 +3640,30 @@
         <v>8</v>
       </c>
       <c r="E77" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F77" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G77">
         <v>1</v>
       </c>
       <c r="H77" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I77" t="s">
         <v>29</v>
       </c>
       <c r="J77" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>417</v>
       </c>
       <c r="B78" s="42" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
@@ -3680,30 +3672,30 @@
         <v>8</v>
       </c>
       <c r="E78" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F78" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G78">
         <v>1</v>
       </c>
       <c r="H78" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I78" t="s">
         <v>29</v>
       </c>
       <c r="J78" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>424</v>
       </c>
       <c r="B79" s="43" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C79" t="s">
         <v>6</v>
@@ -3715,27 +3707,27 @@
         <v>24</v>
       </c>
       <c r="F79" t="s">
+        <v>248</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="H79" t="s">
+        <v>151</v>
+      </c>
+      <c r="I79" t="s">
+        <v>29</v>
+      </c>
+      <c r="J79" t="s">
         <v>249</v>
       </c>
-      <c r="G79">
-        <v>1</v>
-      </c>
-      <c r="H79" t="s">
-        <v>152</v>
-      </c>
-      <c r="I79" t="s">
-        <v>29</v>
-      </c>
-      <c r="J79" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10">
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>647</v>
       </c>
       <c r="B80" s="44" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C80" t="s">
         <v>6</v>
@@ -3753,36 +3745,36 @@
         <v>1</v>
       </c>
       <c r="H80" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I80" t="s">
         <v>29</v>
       </c>
       <c r="J80" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1" display="https://leetcode.com/problems/merge-k-sorted-lists" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B7" r:id="rId2" display="https://leetcode.com/problems/3sum" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://leetcode.com/problems/median-of-two-sorted-arrays" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B14" r:id="rId4" display="https://leetcode.com/problems/rotate-image" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B17" r:id="rId5" display="https://leetcode.com/problems/spiral-matrix" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="J21" r:id="rId6" display="https://leetcode.com/problems/unique-paths/discuss/1581998/C%2B%2BPython-5-Simple-Solutions-w-Explanation-or-Optimization-from-Brute-Force-to-DP-to-Math" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="J22" r:id="rId7" display="https://leetcode.com/problems/unique-paths/discuss/1581998/C%2B%2BPython-5-Simple-Solutions-w-Explanation-or-Optimization-from-Brute-Force-to-DP-to-Math" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="J30" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B37" r:id="rId9" display="https://leetcode.com/problems/longest-consecutive-sequence" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="J38" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="J39" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="J50" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B64" r:id="rId13" display="https://leetcode.com/problems/meeting-rooms" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B65" r:id="rId14" display="https://leetcode.com/problems/meeting-rooms-ii" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B66" r:id="rId15" display="https://leetcode.com/problems/graph-valid-tree" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B68" r:id="rId16" display="https://www.cnblogs.com/grandyang/p/5250200.html" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B69" r:id="rId17" display="https://www.cnblogs.com/grandyang/p/5265628.html" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B73" r:id="rId18" display="https://www.cnblogs.com/grandyang/p/5138186.html" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B11" r:id="rId1" display="https://leetcode.com/problems/merge-k-sorted-lists"/>
+    <hyperlink ref="B7" r:id="rId2" display="https://leetcode.com/problems/3sum"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://leetcode.com/problems/median-of-two-sorted-arrays"/>
+    <hyperlink ref="B14" r:id="rId4" display="https://leetcode.com/problems/rotate-image"/>
+    <hyperlink ref="B17" r:id="rId5" display="https://leetcode.com/problems/spiral-matrix"/>
+    <hyperlink ref="J21" r:id="rId6" display="https://leetcode.com/problems/unique-paths/discuss/1581998/C%2B%2BPython-5-Simple-Solutions-w-Explanation-or-Optimization-from-Brute-Force-to-DP-to-Math"/>
+    <hyperlink ref="J22" r:id="rId7" display="https://leetcode.com/problems/unique-paths/discuss/1581998/C%2B%2BPython-5-Simple-Solutions-w-Explanation-or-Optimization-from-Brute-Force-to-DP-to-Math"/>
+    <hyperlink ref="J30" r:id="rId8"/>
+    <hyperlink ref="B37" r:id="rId9" display="https://leetcode.com/problems/longest-consecutive-sequence"/>
+    <hyperlink ref="J38" r:id="rId10"/>
+    <hyperlink ref="J39" r:id="rId11"/>
+    <hyperlink ref="J50" r:id="rId12"/>
+    <hyperlink ref="B64" r:id="rId13" display="https://leetcode.com/problems/meeting-rooms"/>
+    <hyperlink ref="B65" r:id="rId14" display="https://leetcode.com/problems/meeting-rooms-ii"/>
+    <hyperlink ref="B66" r:id="rId15" display="https://leetcode.com/problems/graph-valid-tree"/>
+    <hyperlink ref="B68" r:id="rId16" display="https://www.cnblogs.com/grandyang/p/5250200.html"/>
+    <hyperlink ref="B69" r:id="rId17" display="https://www.cnblogs.com/grandyang/p/5265628.html"/>
+    <hyperlink ref="B73" r:id="rId18" display="https://www.cnblogs.com/grandyang/p/5138186.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>

</xml_diff>

<commit_message>
Add 59 Update 54,55
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="252">
   <si>
     <t>Question Number</t>
   </si>
@@ -171,9 +171,6 @@
   </si>
   <si>
     <t>Insert Interval</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/insert-interval/discuss/844523/C%2B%2B-Super-Clean-Clear-Short-and-Simple-Solution-O(n)-time-O(1)-space</t>
   </si>
   <si>
     <t>Unique Paths</t>
@@ -204,9 +201,6 @@
     <t>https://leetcode.com/problems/set-matrix-zeroes/discuss/1400849/Set-Matrix-Zeroes-oror-2-Approach-w-Explanation-oror-C%2B%2B-or-Python-or-Java</t>
   </si>
   <si>
-    <t>re-do understand</t>
-  </si>
-  <si>
     <t>Minimum Window Substring</t>
   </si>
   <si>
@@ -274,7 +268,7 @@
   </si>
   <si>
     <t>OnePass, Brute,DP</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Binary Tree Maximum Path Sum</t>
@@ -284,71 +278,71 @@
   </si>
   <si>
     <t>String</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Longest Consecutive Sequence</t>
   </si>
   <si>
     <t>Study how is solution O(n)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Clone Graph</t>
   </si>
   <si>
     <t>Medium</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Graph</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>HashMap,DFS,BFS</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>need to understand</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>https://leetcode.com/problems/clone-graph/discuss/1793212/C%2B%2Bor-Detailed-Explanation-w-DFS-and-BFS-or-Commented-code-with-extra-Test-Case</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Word Break</t>
   </si>
   <si>
     <t>String</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>HashMap,DP</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>https://leetcode.com/problems/word-break/discuss/43814/C%2B%2B-Dynamic-Programming-simple-and-fast-solution-(4ms)-with-optimization</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>need to understand</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Linked List Cycle</t>
   </si>
   <si>
     <t>Easy</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>C++</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>LinkedList</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>https://leetcode.com/problems/linked-list-cycle/discuss/1829489/C%2B%2B-oror-Easy-To-Understand-oror-2-Pointer-oror-Fast-and-Slow</t>
@@ -358,7 +352,7 @@
   </si>
   <si>
     <t>TwoPoint(Floyd’s Cycle-Finding Algorithm)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>TwoPoint</t>
@@ -371,23 +365,23 @@
   </si>
   <si>
     <t>Medium</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>C++</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Array</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>DP</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>need to understand</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>https://leetcode.com/problems/maximum-product-subarray/discuss/183483/JavaC%2B%2BPython-it-can-be-more-simple</t>
@@ -481,22 +475,22 @@
   </si>
   <si>
     <t>Course Schedule</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Tree</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Need to understand</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>https://leetcode.com/problems/implement-trie-prefix-tree/discuss/58945/Share-my-C%2B%2B-solutioneasy-to-understand</t>
   </si>
   <si>
     <t>Implement Trie (Prefix Tree)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Design Add and Search Words Data Structure</t>
@@ -509,11 +503,11 @@
   </si>
   <si>
     <t>Hard</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Backtracking, DFS</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>https://leetcode.com/problems/word-search-ii/discuss/878708/C%2B%2BPython-Backtracking-with-Trie-Clean-and-Concise</t>
@@ -526,54 +520,54 @@
   </si>
   <si>
     <t>Medium</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>C++</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Array</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Easy</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>C++</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Hashmap</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Contains Duplicate</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Invert Binary Tree</t>
   </si>
   <si>
     <t>Easy</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>C++</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Tree</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Queue</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Can to understad BFS,DFS</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>https://leetcode.com/problems/invert-binary-tree/discuss/62891/C%2B%2B-no-recursion-clean-BFS-solution</t>
@@ -583,61 +577,61 @@
   </si>
   <si>
     <t>Medium</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>C++</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Tree</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Need to understant others answer</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Lowest Common Ancestor of a Binary Search Tree</t>
   </si>
   <si>
     <t>Easy</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>C++</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree/discuss/64980/C%2B%2B-Recursive-and-Iterative</t>
   </si>
   <si>
     <t>Iterative, Recursion</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Product of Array Except Self</t>
   </si>
   <si>
     <t>Medium</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Array</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Prefix and Suffix</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">Need to understand Prefix </t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>https://leetcode.com/problems/product-of-array-except-self/discuss/65627/O(n)-time-and-O(1)-space-C%2B%2B-solution-with-explanation
 https://leetcode.com/problems/product-of-array-except-self/discuss/1610450/Attention-No-One-Going-to-Explain-like-this</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>https://leetcode.com/problems/valid-anagram/discuss/66519/2-C%2B%2B-Solutions-with-Explanations</t>
@@ -647,19 +641,19 @@
   </si>
   <si>
     <t>Easy</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>C++</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>String</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Hashmap</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Meeting Rooms</t>
@@ -678,110 +672,110 @@
   </si>
   <si>
     <t>Missing Number</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Alien Dictionary 另类字典</t>
   </si>
   <si>
     <t>Hard</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>C++</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>https://www.cnblogs.com/grandyang/p/5250200.html</t>
   </si>
   <si>
     <t>Understand bit manipulation</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Encode and Decode Strings 加码解码字符串</t>
   </si>
   <si>
     <t>Medium</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>C++</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Find Median from Data Stream</t>
   </si>
   <si>
     <t>Hard</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>C++</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Design</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>https://leetcode.com/problems/find-median-from-data-stream/discuss/1330646/C%2B%2BJavaPython-MinHeap-MaxHeap-Solution-Picture-explain-Clean-and-Concise</t>
   </si>
   <si>
     <t>Priority_queue</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Serialize and Deserialize Binary Tree</t>
   </si>
   <si>
     <t>C++</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Tree</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Longest Increasing Subsequence</t>
   </si>
   <si>
     <t>Medium</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>C++</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Array</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>DP, Binary Tree</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>https://leetcode.com/problems/longest-increasing-subsequence/discuss/1326308/C%2B%2BPython-DP-Binary-Search-BIT-Solutions-Picture-explain-O(NlogN)</t>
   </si>
   <si>
     <t>Need to understand other</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>https://www.cnblogs.com/grandyang/p/5138186.html</t>
   </si>
   <si>
     <t>Need to understand</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>DP</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Array</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Coin Change 硬币找零</t>
@@ -845,22 +839,38 @@
   </si>
   <si>
     <t>Backtracking</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>https://ithelp.ithome.com.tw/users/20119871/ironman/2210?page=1</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>must learn</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Greedy, DP</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/insert-interval/discuss/844523/C%2B%2B-Super-Clean-Clear-Short-and-Simple-Solution-O(n)-time-O(1)-space</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spiral Matrix II</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Matrix</t>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="40" x14ac:knownFonts="1">
+  <fonts count="38" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -896,18 +906,6 @@
       <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF212121"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF212121"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -1148,7 +1146,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1171,8 +1169,8 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1189,23 +1187,21 @@
     <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="36" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1521,10 +1517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J80"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
@@ -1869,7 +1865,7 @@
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -1953,13 +1949,13 @@
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I16" t="s">
         <v>28</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1992,7 +1988,7 @@
       <c r="A18">
         <v>55</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C18" t="s">
@@ -2005,13 +2001,10 @@
         <v>9</v>
       </c>
       <c r="F18" t="s">
-        <v>40</v>
+        <v>248</v>
       </c>
       <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18" t="s">
-        <v>59</v>
+        <v>2</v>
       </c>
       <c r="I18" t="s">
         <v>28</v>
@@ -2021,7 +2014,7 @@
       <c r="A19">
         <v>56</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C19" t="s">
@@ -2037,7 +2030,7 @@
         <v>47</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I19" t="s">
         <v>28</v>
@@ -2047,7 +2040,7 @@
       <c r="A20">
         <v>57</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C20" t="s">
@@ -2060,21 +2053,21 @@
         <v>9</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I20" t="s">
         <v>28</v>
       </c>
-      <c r="J20" t="s">
-        <v>49</v>
+      <c r="J20" s="6" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>59</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>50</v>
+      <c r="B21" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -2083,7 +2076,7 @@
         <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F21" t="s">
         <v>25</v>
@@ -2092,21 +2085,21 @@
         <v>1</v>
       </c>
       <c r="H21" t="s">
+        <v>51</v>
+      </c>
+      <c r="I21" t="s">
+        <v>28</v>
+      </c>
+      <c r="J21" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="I21" t="s">
-        <v>28</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>62</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>50</v>
+      <c r="B22" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -2115,7 +2108,7 @@
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F22" t="s">
         <v>25</v>
@@ -2124,21 +2117,21 @@
         <v>1</v>
       </c>
       <c r="H22" t="s">
+        <v>51</v>
+      </c>
+      <c r="I22" t="s">
+        <v>28</v>
+      </c>
+      <c r="J22" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="I22" t="s">
-        <v>28</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>70</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>54</v>
+      <c r="B23" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="C23" t="s">
         <v>19</v>
@@ -2147,7 +2140,7 @@
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F23" t="s">
         <v>25</v>
@@ -2163,8 +2156,8 @@
       <c r="A24">
         <v>73</v>
       </c>
-      <c r="B24" s="14" t="s">
-        <v>55</v>
+      <c r="B24" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
@@ -2176,27 +2169,27 @@
         <v>9</v>
       </c>
       <c r="F24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
         <v>56</v>
       </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24" t="s">
         <v>57</v>
-      </c>
-      <c r="I24" t="s">
-        <v>28</v>
-      </c>
-      <c r="J24" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>76</v>
       </c>
-      <c r="B25" s="15" t="s">
-        <v>60</v>
+      <c r="B25" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
@@ -2218,8 +2211,8 @@
       <c r="A26">
         <v>79</v>
       </c>
-      <c r="B26" s="16" t="s">
-        <v>61</v>
+      <c r="B26" s="14" t="s">
+        <v>59</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
@@ -2231,7 +2224,7 @@
         <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -2243,15 +2236,15 @@
         <v>28</v>
       </c>
       <c r="J26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>91</v>
       </c>
-      <c r="B27" s="16" t="s">
-        <v>64</v>
+      <c r="B27" s="14" t="s">
+        <v>62</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
@@ -2273,8 +2266,8 @@
       <c r="A28">
         <v>98</v>
       </c>
-      <c r="B28" s="17" t="s">
-        <v>65</v>
+      <c r="B28" s="15" t="s">
+        <v>63</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -2283,30 +2276,30 @@
         <v>8</v>
       </c>
       <c r="E28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
         <v>66</v>
       </c>
-      <c r="F28" t="s">
+      <c r="I28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" t="s">
         <v>67</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-      <c r="H28" t="s">
-        <v>68</v>
-      </c>
-      <c r="I28" t="s">
-        <v>28</v>
-      </c>
-      <c r="J28" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>94</v>
       </c>
-      <c r="B29" s="17" t="s">
-        <v>70</v>
+      <c r="B29" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="C29" t="s">
         <v>19</v>
@@ -2315,24 +2308,24 @@
         <v>8</v>
       </c>
       <c r="E29" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29" t="s">
         <v>66</v>
-      </c>
-      <c r="F29" t="s">
-        <v>71</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="H29" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>100</v>
       </c>
-      <c r="B30" s="17" t="s">
-        <v>72</v>
+      <c r="B30" s="15" t="s">
+        <v>70</v>
       </c>
       <c r="C30" t="s">
         <v>19</v>
@@ -2341,7 +2334,7 @@
         <v>8</v>
       </c>
       <c r="E30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F30" t="s">
         <v>35</v>
@@ -2353,15 +2346,15 @@
         <v>28</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>102</v>
       </c>
-      <c r="B31" s="18" t="s">
-        <v>74</v>
+      <c r="B31" s="16" t="s">
+        <v>72</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
@@ -2370,30 +2363,30 @@
         <v>8</v>
       </c>
       <c r="E31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F31" t="s">
+        <v>73</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
         <v>75</v>
       </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31" t="s">
-        <v>77</v>
-      </c>
       <c r="I31" t="s">
         <v>28</v>
       </c>
       <c r="J31" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>104</v>
       </c>
-      <c r="B32" s="19" t="s">
-        <v>78</v>
+      <c r="B32" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="C32" t="s">
         <v>19</v>
@@ -2402,7 +2395,7 @@
         <v>8</v>
       </c>
       <c r="E32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F32" t="s">
         <v>35</v>
@@ -2418,8 +2411,8 @@
       <c r="A33">
         <v>105</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>79</v>
+      <c r="B33" s="17" t="s">
+        <v>77</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
@@ -2428,21 +2421,21 @@
         <v>8</v>
       </c>
       <c r="E33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I33" t="s">
         <v>28</v>
       </c>
       <c r="J33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>121</v>
       </c>
-      <c r="B34" s="19" t="s">
-        <v>81</v>
+      <c r="B34" s="17" t="s">
+        <v>79</v>
       </c>
       <c r="C34" t="s">
         <v>19</v>
@@ -2454,7 +2447,7 @@
         <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G34">
         <v>2</v>
@@ -2467,8 +2460,8 @@
       <c r="A35">
         <v>124</v>
       </c>
-      <c r="B35" s="20" t="s">
-        <v>83</v>
+      <c r="B35" s="18" t="s">
+        <v>81</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
@@ -2477,7 +2470,7 @@
         <v>8</v>
       </c>
       <c r="E35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I35" t="s">
         <v>28</v>
@@ -2487,8 +2480,8 @@
       <c r="A36">
         <v>125</v>
       </c>
-      <c r="B36" s="21" t="s">
-        <v>84</v>
+      <c r="B36" s="19" t="s">
+        <v>82</v>
       </c>
       <c r="C36" t="s">
         <v>19</v>
@@ -2497,7 +2490,7 @@
         <v>8</v>
       </c>
       <c r="E36" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G36">
         <v>1</v>
@@ -2511,7 +2504,7 @@
         <v>128</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C37" t="s">
         <v>19</v>
@@ -2526,7 +2519,7 @@
         <v>1</v>
       </c>
       <c r="H37" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I37" t="s">
         <v>28</v>
@@ -2536,114 +2529,114 @@
       <c r="A38">
         <v>133</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" t="s">
         <v>88</v>
       </c>
-      <c r="C38" t="s">
+      <c r="F38" t="s">
         <v>89</v>
       </c>
-      <c r="D38" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38" t="s">
         <v>90</v>
       </c>
-      <c r="F38" t="s">
+      <c r="I38" t="s">
+        <v>28</v>
+      </c>
+      <c r="J38" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
-      <c r="H38" t="s">
-        <v>92</v>
-      </c>
-      <c r="I38" t="s">
-        <v>28</v>
-      </c>
-      <c r="J38" s="6" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>139</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" t="s">
+        <v>93</v>
+      </c>
+      <c r="F39" t="s">
         <v>94</v>
       </c>
-      <c r="C39" t="s">
-        <v>89</v>
-      </c>
-      <c r="D39" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
+        <v>96</v>
+      </c>
+      <c r="I39" t="s">
+        <v>28</v>
+      </c>
+      <c r="J39" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="F39" t="s">
-        <v>96</v>
-      </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
-      <c r="H39" t="s">
-        <v>98</v>
-      </c>
-      <c r="I39" t="s">
-        <v>28</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>141</v>
       </c>
-      <c r="B40" s="23" t="s">
+      <c r="B40" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" t="s">
         <v>99</v>
       </c>
-      <c r="C40" t="s">
+      <c r="E40" t="s">
         <v>100</v>
       </c>
-      <c r="D40" t="s">
+      <c r="F40" t="s">
+        <v>103</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="I40" t="s">
+        <v>28</v>
+      </c>
+      <c r="J40" t="s">
         <v>101</v>
-      </c>
-      <c r="E40" t="s">
-        <v>102</v>
-      </c>
-      <c r="F40" t="s">
-        <v>105</v>
-      </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="I40" t="s">
-        <v>28</v>
-      </c>
-      <c r="J40" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>143</v>
       </c>
-      <c r="B41" s="24" t="s">
+      <c r="B41" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E41" t="s">
+        <v>100</v>
+      </c>
+      <c r="F41" t="s">
         <v>104</v>
       </c>
-      <c r="C41" t="s">
-        <v>89</v>
-      </c>
-      <c r="D41" t="s">
-        <v>101</v>
-      </c>
-      <c r="E41" t="s">
-        <v>102</v>
-      </c>
-      <c r="F41" t="s">
-        <v>106</v>
-      </c>
       <c r="G41">
         <v>1</v>
       </c>
@@ -2651,7 +2644,7 @@
         <v>28</v>
       </c>
       <c r="J41" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
@@ -2659,74 +2652,74 @@
         <v>152</v>
       </c>
       <c r="B42" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C42" t="s">
+        <v>107</v>
+      </c>
+      <c r="D42" t="s">
         <v>108</v>
       </c>
-      <c r="C42" t="s">
+      <c r="E42" t="s">
         <v>109</v>
       </c>
-      <c r="D42" t="s">
+      <c r="F42" t="s">
         <v>110</v>
       </c>
-      <c r="E42" t="s">
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42" t="s">
         <v>111</v>
       </c>
-      <c r="F42" t="s">
+      <c r="I42" t="s">
+        <v>28</v>
+      </c>
+      <c r="J42" t="s">
         <v>112</v>
-      </c>
-      <c r="G42">
-        <v>1</v>
-      </c>
-      <c r="H42" t="s">
-        <v>113</v>
-      </c>
-      <c r="I42" t="s">
-        <v>28</v>
-      </c>
-      <c r="J42" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2114</v>
       </c>
-      <c r="B43" s="25" t="s">
-        <v>115</v>
+      <c r="B43" s="23" t="s">
+        <v>113</v>
       </c>
       <c r="C43" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D43" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E43" t="s">
         <v>23</v>
       </c>
       <c r="F43" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G43">
         <v>1</v>
       </c>
       <c r="J43" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2236</v>
       </c>
-      <c r="B44" s="26" t="s">
-        <v>118</v>
+      <c r="B44" s="24" t="s">
+        <v>116</v>
       </c>
       <c r="C44" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D44" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E44" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G44">
         <v>1</v>
@@ -2736,8 +2729,8 @@
       <c r="A45">
         <v>1023</v>
       </c>
-      <c r="B45" s="27" t="s">
-        <v>119</v>
+      <c r="B45" s="25" t="s">
+        <v>117</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
@@ -2752,15 +2745,15 @@
         <v>1</v>
       </c>
       <c r="J45" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>831</v>
       </c>
-      <c r="B46" s="27" t="s">
-        <v>121</v>
+      <c r="B46" s="25" t="s">
+        <v>119</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
@@ -2775,7 +2768,7 @@
         <v>1</v>
       </c>
       <c r="J46" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
@@ -2783,7 +2776,7 @@
         <v>153</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
@@ -2801,7 +2794,7 @@
         <v>1</v>
       </c>
       <c r="H47" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I47" t="s">
         <v>28</v>
@@ -2811,8 +2804,8 @@
       <c r="A48">
         <v>190</v>
       </c>
-      <c r="B48" s="28" t="s">
-        <v>125</v>
+      <c r="B48" s="26" t="s">
+        <v>123</v>
       </c>
       <c r="C48" t="s">
         <v>19</v>
@@ -2821,7 +2814,7 @@
         <v>8</v>
       </c>
       <c r="E48" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F48" t="s">
         <v>36</v>
@@ -2830,21 +2823,21 @@
         <v>1</v>
       </c>
       <c r="H48" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I48" t="s">
         <v>28</v>
       </c>
       <c r="J48" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>191</v>
       </c>
-      <c r="B49" s="28" t="s">
-        <v>129</v>
+      <c r="B49" s="26" t="s">
+        <v>127</v>
       </c>
       <c r="C49" t="s">
         <v>19</v>
@@ -2853,10 +2846,10 @@
         <v>8</v>
       </c>
       <c r="E49" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F49" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G49">
         <v>1</v>
@@ -2869,8 +2862,8 @@
       <c r="A50">
         <v>198</v>
       </c>
-      <c r="B50" s="29" t="s">
-        <v>131</v>
+      <c r="B50" s="27" t="s">
+        <v>129</v>
       </c>
       <c r="C50" t="s">
         <v>6</v>
@@ -2888,21 +2881,21 @@
         <v>1</v>
       </c>
       <c r="H50" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I50" t="s">
         <v>28</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>200</v>
       </c>
-      <c r="B51" s="30" t="s">
-        <v>133</v>
+      <c r="B51" s="28" t="s">
+        <v>131</v>
       </c>
       <c r="C51" t="s">
         <v>6</v>
@@ -2914,27 +2907,27 @@
         <v>9</v>
       </c>
       <c r="F51" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G51">
         <v>1</v>
       </c>
       <c r="H51" t="s">
+        <v>133</v>
+      </c>
+      <c r="I51" t="s">
+        <v>28</v>
+      </c>
+      <c r="J51" t="s">
         <v>135</v>
-      </c>
-      <c r="I51" t="s">
-        <v>28</v>
-      </c>
-      <c r="J51" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>206</v>
       </c>
-      <c r="B52" s="30" t="s">
-        <v>138</v>
+      <c r="B52" s="28" t="s">
+        <v>136</v>
       </c>
       <c r="C52" t="s">
         <v>19</v>
@@ -2946,7 +2939,7 @@
         <v>14</v>
       </c>
       <c r="F52" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G52">
         <v>1</v>
@@ -2955,7 +2948,7 @@
         <v>28</v>
       </c>
       <c r="J52" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
@@ -2963,7 +2956,7 @@
         <v>207</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C53" t="s">
         <v>6</v>
@@ -2972,27 +2965,27 @@
         <v>8</v>
       </c>
       <c r="E53" t="s">
+        <v>139</v>
+      </c>
+      <c r="F53" t="s">
+        <v>132</v>
+      </c>
+      <c r="H53" t="s">
+        <v>140</v>
+      </c>
+      <c r="I53" t="s">
+        <v>28</v>
+      </c>
+      <c r="J53" t="s">
         <v>141</v>
-      </c>
-      <c r="F53" t="s">
-        <v>134</v>
-      </c>
-      <c r="H53" t="s">
-        <v>142</v>
-      </c>
-      <c r="I53" t="s">
-        <v>28</v>
-      </c>
-      <c r="J53" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>208</v>
       </c>
-      <c r="B54" s="31" t="s">
-        <v>148</v>
+      <c r="B54" s="29" t="s">
+        <v>146</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
@@ -3001,24 +2994,24 @@
         <v>8</v>
       </c>
       <c r="E54" t="s">
+        <v>143</v>
+      </c>
+      <c r="H54" t="s">
+        <v>144</v>
+      </c>
+      <c r="I54" t="s">
+        <v>28</v>
+      </c>
+      <c r="J54" t="s">
         <v>145</v>
-      </c>
-      <c r="H54" t="s">
-        <v>146</v>
-      </c>
-      <c r="I54" t="s">
-        <v>28</v>
-      </c>
-      <c r="J54" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>211</v>
       </c>
-      <c r="B55" s="32" t="s">
-        <v>149</v>
+      <c r="B55" s="30" t="s">
+        <v>147</v>
       </c>
       <c r="C55" t="s">
         <v>6</v>
@@ -3027,77 +3020,77 @@
         <v>8</v>
       </c>
       <c r="E55" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H55" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I55" t="s">
         <v>28</v>
       </c>
       <c r="J55" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>212</v>
       </c>
-      <c r="B56" s="32" t="s">
+      <c r="B56" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="C56" t="s">
+        <v>150</v>
+      </c>
+      <c r="D56" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" t="s">
+        <v>143</v>
+      </c>
+      <c r="F56" t="s">
         <v>151</v>
       </c>
-      <c r="C56" t="s">
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56" t="s">
+        <v>144</v>
+      </c>
+      <c r="I56" t="s">
+        <v>28</v>
+      </c>
+      <c r="J56" t="s">
         <v>152</v>
-      </c>
-      <c r="D56" t="s">
-        <v>8</v>
-      </c>
-      <c r="E56" t="s">
-        <v>145</v>
-      </c>
-      <c r="F56" t="s">
-        <v>153</v>
-      </c>
-      <c r="G56">
-        <v>1</v>
-      </c>
-      <c r="H56" t="s">
-        <v>146</v>
-      </c>
-      <c r="I56" t="s">
-        <v>28</v>
-      </c>
-      <c r="J56" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>213</v>
       </c>
-      <c r="B57" s="33" t="s">
+      <c r="B57" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="C57" t="s">
+        <v>155</v>
+      </c>
+      <c r="D57" t="s">
         <v>156</v>
       </c>
-      <c r="C57" t="s">
+      <c r="E57" t="s">
         <v>157</v>
       </c>
-      <c r="D57" t="s">
-        <v>158</v>
-      </c>
-      <c r="E57" t="s">
-        <v>159</v>
-      </c>
       <c r="G57">
         <v>1</v>
       </c>
       <c r="H57" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I57" t="s">
         <v>28</v>
       </c>
       <c r="J57" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
@@ -3105,19 +3098,19 @@
         <v>217</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C58" t="s">
+        <v>158</v>
+      </c>
+      <c r="D58" t="s">
+        <v>159</v>
+      </c>
+      <c r="E58" t="s">
+        <v>157</v>
+      </c>
+      <c r="F58" t="s">
         <v>160</v>
-      </c>
-      <c r="D58" t="s">
-        <v>161</v>
-      </c>
-      <c r="E58" t="s">
-        <v>159</v>
-      </c>
-      <c r="F58" t="s">
-        <v>162</v>
       </c>
       <c r="G58">
         <v>1</v>
@@ -3130,58 +3123,58 @@
       <c r="A59">
         <v>226</v>
       </c>
-      <c r="B59" s="34" t="s">
+      <c r="B59" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="C59" t="s">
+        <v>163</v>
+      </c>
+      <c r="D59" t="s">
         <v>164</v>
       </c>
-      <c r="C59" t="s">
+      <c r="E59" t="s">
         <v>165</v>
       </c>
-      <c r="D59" t="s">
+      <c r="F59" t="s">
         <v>166</v>
       </c>
-      <c r="E59" t="s">
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59" t="s">
         <v>167</v>
       </c>
-      <c r="F59" t="s">
+      <c r="I59" t="s">
+        <v>28</v>
+      </c>
+      <c r="J59" t="s">
         <v>168</v>
-      </c>
-      <c r="G59">
-        <v>1</v>
-      </c>
-      <c r="H59" t="s">
-        <v>169</v>
-      </c>
-      <c r="I59" t="s">
-        <v>28</v>
-      </c>
-      <c r="J59" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>230</v>
       </c>
-      <c r="B60" s="35" t="s">
+      <c r="B60" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="C60" t="s">
+        <v>170</v>
+      </c>
+      <c r="D60" t="s">
         <v>171</v>
       </c>
-      <c r="C60" t="s">
+      <c r="E60" t="s">
         <v>172</v>
       </c>
-      <c r="D60" t="s">
+      <c r="F60" t="s">
+        <v>166</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60" t="s">
         <v>173</v>
-      </c>
-      <c r="E60" t="s">
-        <v>174</v>
-      </c>
-      <c r="F60" t="s">
-        <v>168</v>
-      </c>
-      <c r="G60">
-        <v>1</v>
-      </c>
-      <c r="H60" t="s">
-        <v>175</v>
       </c>
       <c r="I60" t="s">
         <v>28</v>
@@ -3191,61 +3184,61 @@
       <c r="A61">
         <v>235</v>
       </c>
-      <c r="B61" s="36" t="s">
+      <c r="B61" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="C61" t="s">
+        <v>175</v>
+      </c>
+      <c r="D61" t="s">
         <v>176</v>
       </c>
-      <c r="C61" t="s">
+      <c r="E61" t="s">
+        <v>143</v>
+      </c>
+      <c r="F61" t="s">
+        <v>178</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="I61" t="s">
+        <v>28</v>
+      </c>
+      <c r="J61" t="s">
         <v>177</v>
-      </c>
-      <c r="D61" t="s">
-        <v>178</v>
-      </c>
-      <c r="E61" t="s">
-        <v>145</v>
-      </c>
-      <c r="F61" t="s">
-        <v>180</v>
-      </c>
-      <c r="G61">
-        <v>1</v>
-      </c>
-      <c r="I61" t="s">
-        <v>28</v>
-      </c>
-      <c r="J61" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>238</v>
       </c>
-      <c r="B62" s="37" t="s">
+      <c r="B62" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="C62" t="s">
+        <v>180</v>
+      </c>
+      <c r="D62" t="s">
+        <v>99</v>
+      </c>
+      <c r="E62" t="s">
         <v>181</v>
       </c>
-      <c r="C62" t="s">
+      <c r="F62" t="s">
         <v>182</v>
       </c>
-      <c r="D62" t="s">
-        <v>101</v>
-      </c>
-      <c r="E62" t="s">
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62" t="s">
         <v>183</v>
       </c>
-      <c r="F62" t="s">
+      <c r="I62" t="s">
+        <v>28</v>
+      </c>
+      <c r="J62" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="G62">
-        <v>1</v>
-      </c>
-      <c r="H62" t="s">
-        <v>185</v>
-      </c>
-      <c r="I62" t="s">
-        <v>28</v>
-      </c>
-      <c r="J62" s="5" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
@@ -3253,20 +3246,20 @@
         <v>242</v>
       </c>
       <c r="B63" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C63" t="s">
+        <v>187</v>
+      </c>
+      <c r="D63" t="s">
         <v>188</v>
       </c>
-      <c r="C63" t="s">
+      <c r="E63" t="s">
         <v>189</v>
       </c>
-      <c r="D63" t="s">
+      <c r="F63" t="s">
         <v>190</v>
       </c>
-      <c r="E63" t="s">
-        <v>191</v>
-      </c>
-      <c r="F63" t="s">
-        <v>192</v>
-      </c>
       <c r="G63">
         <v>1</v>
       </c>
@@ -3274,15 +3267,15 @@
         <v>28</v>
       </c>
       <c r="J63" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>252</v>
       </c>
-      <c r="B64" s="38" t="s">
-        <v>193</v>
+      <c r="B64" s="36" t="s">
+        <v>191</v>
       </c>
       <c r="C64" t="s">
         <v>19</v>
@@ -3297,21 +3290,21 @@
         <v>1</v>
       </c>
       <c r="H64" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I64" t="s">
         <v>28</v>
       </c>
       <c r="J64" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>253</v>
       </c>
-      <c r="B65" s="38" t="s">
-        <v>196</v>
+      <c r="B65" s="36" t="s">
+        <v>194</v>
       </c>
       <c r="C65" t="s">
         <v>6</v>
@@ -3323,7 +3316,7 @@
         <v>9</v>
       </c>
       <c r="H65" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I65" t="s">
         <v>28</v>
@@ -3333,8 +3326,8 @@
       <c r="A66">
         <v>261</v>
       </c>
-      <c r="B66" s="38" t="s">
-        <v>197</v>
+      <c r="B66" s="36" t="s">
+        <v>195</v>
       </c>
       <c r="C66" t="s">
         <v>6</v>
@@ -3343,10 +3336,10 @@
         <v>8</v>
       </c>
       <c r="E66" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H66" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I66" t="s">
         <v>28</v>
@@ -3357,7 +3350,7 @@
         <v>268</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C67" t="s">
         <v>19</v>
@@ -3372,7 +3365,7 @@
         <v>1</v>
       </c>
       <c r="H67" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I67" t="s">
         <v>28</v>
@@ -3382,34 +3375,34 @@
       <c r="A68">
         <v>269</v>
       </c>
-      <c r="B68" s="39" t="s">
+      <c r="B68" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="C68" t="s">
+        <v>198</v>
+      </c>
+      <c r="D68" t="s">
         <v>199</v>
       </c>
-      <c r="C68" t="s">
+      <c r="I68" t="s">
+        <v>28</v>
+      </c>
+      <c r="J68" t="s">
         <v>200</v>
-      </c>
-      <c r="D68" t="s">
-        <v>201</v>
-      </c>
-      <c r="I68" t="s">
-        <v>28</v>
-      </c>
-      <c r="J68" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>271</v>
       </c>
-      <c r="B69" s="39" t="s">
+      <c r="B69" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="C69" t="s">
+        <v>203</v>
+      </c>
+      <c r="D69" t="s">
         <v>204</v>
-      </c>
-      <c r="C69" t="s">
-        <v>205</v>
-      </c>
-      <c r="D69" t="s">
-        <v>206</v>
       </c>
       <c r="I69" t="s">
         <v>28</v>
@@ -3419,46 +3412,46 @@
       <c r="A70">
         <v>295</v>
       </c>
-      <c r="B70" s="40" t="s">
+      <c r="B70" s="38" t="s">
+        <v>205</v>
+      </c>
+      <c r="C70" t="s">
+        <v>206</v>
+      </c>
+      <c r="D70" t="s">
         <v>207</v>
       </c>
-      <c r="C70" t="s">
+      <c r="E70" t="s">
         <v>208</v>
       </c>
-      <c r="D70" t="s">
+      <c r="F70" t="s">
+        <v>210</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="I70" t="s">
+        <v>28</v>
+      </c>
+      <c r="J70" t="s">
         <v>209</v>
-      </c>
-      <c r="E70" t="s">
-        <v>210</v>
-      </c>
-      <c r="F70" t="s">
-        <v>212</v>
-      </c>
-      <c r="G70">
-        <v>1</v>
-      </c>
-      <c r="I70" t="s">
-        <v>28</v>
-      </c>
-      <c r="J70" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>297</v>
       </c>
-      <c r="B71" s="41" t="s">
+      <c r="B71" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="C71" t="s">
+        <v>198</v>
+      </c>
+      <c r="D71" t="s">
+        <v>212</v>
+      </c>
+      <c r="E71" t="s">
         <v>213</v>
-      </c>
-      <c r="C71" t="s">
-        <v>200</v>
-      </c>
-      <c r="D71" t="s">
-        <v>214</v>
-      </c>
-      <c r="E71" t="s">
-        <v>215</v>
       </c>
       <c r="I71" t="s">
         <v>28</v>
@@ -3468,101 +3461,101 @@
       <c r="A72">
         <v>300</v>
       </c>
-      <c r="B72" s="42" t="s">
+      <c r="B72" s="40" t="s">
+        <v>214</v>
+      </c>
+      <c r="C72" t="s">
+        <v>215</v>
+      </c>
+      <c r="D72" t="s">
         <v>216</v>
       </c>
-      <c r="C72" t="s">
+      <c r="E72" t="s">
         <v>217</v>
       </c>
-      <c r="D72" t="s">
+      <c r="F72" t="s">
         <v>218</v>
       </c>
-      <c r="E72" t="s">
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72" t="s">
+        <v>220</v>
+      </c>
+      <c r="I72" t="s">
+        <v>28</v>
+      </c>
+      <c r="J72" t="s">
         <v>219</v>
-      </c>
-      <c r="F72" t="s">
-        <v>220</v>
-      </c>
-      <c r="G72">
-        <v>1</v>
-      </c>
-      <c r="H72" t="s">
-        <v>222</v>
-      </c>
-      <c r="I72" t="s">
-        <v>28</v>
-      </c>
-      <c r="J72" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>322</v>
       </c>
-      <c r="B73" s="39" t="s">
-        <v>227</v>
+      <c r="B73" s="37" t="s">
+        <v>225</v>
       </c>
       <c r="C73" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D73" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E73" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F73" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G73">
         <v>1</v>
       </c>
       <c r="H73" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I73" t="s">
         <v>28</v>
       </c>
       <c r="J73" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>323</v>
       </c>
-      <c r="B74" s="43" t="s">
+      <c r="B74" s="41" t="s">
+        <v>226</v>
+      </c>
+      <c r="C74" t="s">
+        <v>87</v>
+      </c>
+      <c r="D74" t="s">
+        <v>99</v>
+      </c>
+      <c r="E74" t="s">
+        <v>139</v>
+      </c>
+      <c r="F74" t="s">
+        <v>227</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="I74" t="s">
+        <v>28</v>
+      </c>
+      <c r="J74" t="s">
         <v>228</v>
-      </c>
-      <c r="C74" t="s">
-        <v>89</v>
-      </c>
-      <c r="D74" t="s">
-        <v>101</v>
-      </c>
-      <c r="E74" t="s">
-        <v>141</v>
-      </c>
-      <c r="F74" t="s">
-        <v>229</v>
-      </c>
-      <c r="G74">
-        <v>1</v>
-      </c>
-      <c r="I74" t="s">
-        <v>28</v>
-      </c>
-      <c r="J74" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>338</v>
       </c>
-      <c r="B75" s="44" t="s">
-        <v>231</v>
+      <c r="B75" s="42" t="s">
+        <v>229</v>
       </c>
       <c r="C75" t="s">
         <v>19</v>
@@ -3571,7 +3564,7 @@
         <v>8</v>
       </c>
       <c r="E75" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F75" t="s">
         <v>25</v>
@@ -3580,21 +3573,21 @@
         <v>1</v>
       </c>
       <c r="H75" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I75" t="s">
         <v>28</v>
       </c>
       <c r="J75" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>347</v>
       </c>
-      <c r="B76" s="45" t="s">
-        <v>234</v>
+      <c r="B76" s="43" t="s">
+        <v>232</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
@@ -3606,27 +3599,27 @@
         <v>9</v>
       </c>
       <c r="F76" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G76">
         <v>1</v>
       </c>
       <c r="H76" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I76" t="s">
         <v>28</v>
       </c>
       <c r="J76" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>371</v>
       </c>
-      <c r="B77" s="45" t="s">
-        <v>238</v>
+      <c r="B77" s="43" t="s">
+        <v>236</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
@@ -3635,30 +3628,30 @@
         <v>8</v>
       </c>
       <c r="E77" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F77" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G77">
         <v>1</v>
       </c>
       <c r="H77" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I77" t="s">
         <v>28</v>
       </c>
       <c r="J77" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>417</v>
       </c>
-      <c r="B78" s="46" t="s">
-        <v>240</v>
+      <c r="B78" s="44" t="s">
+        <v>238</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
@@ -3667,30 +3660,30 @@
         <v>8</v>
       </c>
       <c r="E78" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F78" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G78">
         <v>1</v>
       </c>
       <c r="H78" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I78" t="s">
         <v>28</v>
       </c>
       <c r="J78" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>424</v>
       </c>
-      <c r="B79" s="47" t="s">
-        <v>242</v>
+      <c r="B79" s="45" t="s">
+        <v>240</v>
       </c>
       <c r="C79" t="s">
         <v>6</v>
@@ -3702,27 +3695,27 @@
         <v>23</v>
       </c>
       <c r="F79" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G79">
         <v>1</v>
       </c>
       <c r="H79" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I79" t="s">
         <v>28</v>
       </c>
       <c r="J79" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>647</v>
       </c>
-      <c r="B80" s="48" t="s">
-        <v>245</v>
+      <c r="B80" s="46" t="s">
+        <v>243</v>
       </c>
       <c r="C80" t="s">
         <v>6</v>
@@ -3740,17 +3733,40 @@
         <v>1</v>
       </c>
       <c r="H80" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I80" t="s">
         <v>28</v>
       </c>
       <c r="J80" t="s">
-        <v>246</v>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>59</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C81" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" t="s">
+        <v>251</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1" display="https://leetcode.com/problems/merge-k-sorted-lists"/>
     <hyperlink ref="B7" r:id="rId2" display="https://leetcode.com/problems/3sum"/>
@@ -3771,8 +3787,9 @@
     <hyperlink ref="B69" r:id="rId17" display="https://www.cnblogs.com/grandyang/p/5265628.html"/>
     <hyperlink ref="B73" r:id="rId18" display="https://www.cnblogs.com/grandyang/p/5138186.html"/>
     <hyperlink ref="J16" r:id="rId19"/>
+    <hyperlink ref="J20" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>